<commit_message>
att pagina de processos atrasados
</commit_message>
<xml_diff>
--- a/backend/objetos.xlsx
+++ b/backend/objetos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leozed92-my.sharepoint.com/personal/leozed_leozed92_onmicrosoft_com/Documents/Aplicativos/App GAD SESAU/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="8_{C24DD8E0-50BB-40E4-B648-E8FAFBB74FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6658D95F-9BC4-43D4-94BE-C62FFFBAB40D}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="8_{C24DD8E0-50BB-40E4-B648-E8FAFBB74FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EE27D76-5BCA-4F8E-9171-1F97B213B507}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{92D8D400-3915-4B7A-B5E9-ACA32B0E4BC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>objeto</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>Ambulância Licitatório - Serviço de Transporte Inter-Hospitalar com mão-de-obra</t>
+  </si>
+  <si>
+    <t>0036.020320/2025-35</t>
+  </si>
+  <si>
+    <t>Congresso do Conselho Nacional de Secretario em Brasília</t>
   </si>
 </sst>
 </file>
@@ -246,10 +252,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -569,7 +571,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2FF0CA-3C4D-4BFF-9AA5-A0CFD76751B1}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
@@ -757,6 +759,14 @@
         <v>43</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>